<commit_message>
[Fixed] UI MVVM 세부 내용 수정.
</commit_message>
<xml_diff>
--- a/Assets/Resource/Xlsx/AssetAddress.xlsx
+++ b/Assets/Resource/Xlsx/AssetAddress.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KGA\Documents\GitHub\ProjectOz\Assets\Resource\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KGA\Game\ProjectOz\Assets\Resource\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,7 +38,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Assets/Cube.prefab</t>
+    <t>sword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assets/Resource/sword.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assets/Resource/Cube.prefab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assets/Resource/broom.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>broom</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -367,7 +383,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -385,23 +401,23 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>124</v>
-      </c>
-      <c r="B3">
-        <v>1235</v>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>125</v>
-      </c>
-      <c r="B4">
-        <v>1236</v>
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Update] 타격 VFX 추가
</commit_message>
<xml_diff>
--- a/Assets/Resource/Xlsx/AssetAddress.xlsx
+++ b/Assets/Resource/Xlsx/AssetAddress.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KGA\Documents\GitHub\ProjectOz\Assets\Resource\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KGA\Desktop\Project_Oz\ProjectOz\Assets\Resource\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -122,10 +122,11 @@
     <t>Assets/Resource/Sprite/UISprite/Game_Over_UI.png</t>
   </si>
   <si>
-    <t>Assets/Resource/VFX/PlayerVFX/Hit_vfx/Hit_vfx/Hit_vfx.prefab</t>
-  </si>
-  <si>
     <t>Hit_vfx</t>
+  </si>
+  <si>
+    <t>Assets/Resource/VFX/PlayerVFX/Hit_vfx/Hit_vfx/Holy hit.prefab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -453,7 +454,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -576,10 +577,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>